<commit_message>
Live cycle of the usage implemented
</commit_message>
<xml_diff>
--- a/diagnosis.xlsx
+++ b/diagnosis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/VisualCodeProjects/perceptron/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA097203-66B8-B046-B544-FE73F64D5423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E7BD3-9702-F14F-98BC-A3445BE99C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25300" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -131,13 +131,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -160,6 +188,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1289,11 +1326,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1386,31 +1423,110 @@
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6">
+      <c r="A4" s="9">
         <v>0.5</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
         <v>0</v>
       </c>
       <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>

</xml_diff>

<commit_message>
Přidána historie chyb kvadratického průměru do algoritmu zpětné propagace
</commit_message>
<xml_diff>
--- a/diagnosis.xlsx
+++ b/diagnosis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/VisualCodeProjects/perceptron/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/VisualStudioProjects/MultilayeredNeuralNets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E7BD3-9702-F14F-98BC-A3445BE99C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC1BD39-D0AC-4048-9915-69632F2271EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25300" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="25300" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List 1" sheetId="1" r:id="rId1"/>
@@ -1330,7 +1330,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Softmax example added to Jupyter notebook
</commit_message>
<xml_diff>
--- a/diagnosis.xlsx
+++ b/diagnosis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivo/VisualStudioProjects/MultilayeredNeuralNets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC1BD39-D0AC-4048-9915-69632F2271EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639B8DF4-BD1A-9743-9A71-3986DCE330A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="25300" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="880" windowWidth="25300" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List 1" sheetId="1" r:id="rId1"/>
@@ -1330,7 +1330,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>